<commit_message>
fixed equipment and consumable forms
</commit_message>
<xml_diff>
--- a/accounting/tests/entries.xlsx
+++ b/accounting/tests/entries.xlsx
@@ -14,7 +14,8 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
   <si>
     <t>date</t>
   </si>
@@ -405,7 +406,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -527,6 +528,9 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
       <c r="B7">
         <v>123</v>
       </c>
@@ -541,6 +545,9 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
       <c r="B8">
         <v>123</v>
       </c>
@@ -555,6 +562,9 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
       <c r="B9">
         <v>123</v>
       </c>

</xml_diff>